<commit_message>
Form submission flow case
</commit_message>
<xml_diff>
--- a/Demo_working/src/test/resources/TestData/TestData.xlsx
+++ b/Demo_working/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="17220" windowHeight="4560" tabRatio="845" firstSheet="7" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="2472" windowWidth="16920" windowHeight="8220" tabRatio="706" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="AddPayerNonUsEin" sheetId="14" r:id="rId13"/>
     <sheet name="People" sheetId="15" r:id="rId14"/>
     <sheet name="AddRecipientEin" sheetId="16" r:id="rId15"/>
+    <sheet name="1099MISCdata" sheetId="17" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:Q27"/>
+  <oleSize ref="A1:J11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="130">
   <si>
     <t>TestCases</t>
   </si>
@@ -391,6 +392,39 @@
   </si>
   <si>
     <t>Payers count in manage payer page</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>BusinessName</t>
+  </si>
+  <si>
+    <t>Payer Business name</t>
+  </si>
+  <si>
+    <t>Test0202202120528</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Test0202202134948</t>
+  </si>
+  <si>
+    <t>Test0202202150222</t>
+  </si>
+  <si>
+    <t>Test0202202155851</t>
+  </si>
+  <si>
+    <t>Test0202202160448</t>
+  </si>
+  <si>
+    <t>Test0203202195509</t>
+  </si>
+  <si>
+    <t>Test02032021100108</t>
   </si>
 </sst>
 </file>
@@ -551,6 +585,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -559,9 +596,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -905,13 +939,13 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="5" t="s">
@@ -1258,9 +1292,9 @@
     <col min="2" max="2" customWidth="true" width="21.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>5.46199841E8</v>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>546199841</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1307,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1362,12 +1396,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="28.8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="C9" s="18"/>
+      <c r="C9" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1457,6 +1491,51 @@
       </c>
       <c r="K2" s="12">
         <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="27.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.6640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B4" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>